<commit_message>
Updated options colouring & Calculator buttons
</commit_message>
<xml_diff>
--- a/backend/responses.xlsx
+++ b/backend/responses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding-Experimental\custom-mocktest-website\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinalBackup\Programming\custom-mocktest-website\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E4789-BDB8-458C-8E99-7D0597712090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9415E377-B31E-494E-BF7D-77566A7D0F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -435,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L31"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,36 +481,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>